<commit_message>
Added new scripts for Diag and Test Master
</commit_message>
<xml_diff>
--- a/Documents/Dimensions.xlsx
+++ b/Documents/Dimensions.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Diagnosis" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="99">
   <si>
     <t>Tables</t>
   </si>
@@ -218,13 +219,106 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Identity</t>
+  </si>
+  <si>
+    <t>DiagnosisName</t>
+  </si>
+  <si>
+    <t>_DiagnosisIDOrig</t>
+  </si>
+  <si>
+    <t>IsPanel</t>
+  </si>
+  <si>
+    <t>IsExecutive</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>BIT</t>
+  </si>
+  <si>
+    <t>PanelGroupName</t>
+  </si>
+  <si>
+    <t>ExecutiveGroupName</t>
+  </si>
+  <si>
+    <t>_TestIDOrig</t>
+  </si>
+  <si>
+    <t>_SubTestIDOrig</t>
+  </si>
+  <si>
+    <t>ParentSubTestId</t>
+  </si>
+  <si>
+    <t>TestMaster</t>
+  </si>
+  <si>
+    <t>DiagnosisMaster</t>
+  </si>
+  <si>
+    <t>RangeMin</t>
+  </si>
+  <si>
+    <t>RangeMax</t>
+  </si>
+  <si>
+    <t>OrigDate</t>
+  </si>
+  <si>
+    <t>RangeFromDate</t>
+  </si>
+  <si>
+    <t>RangeToDate</t>
+  </si>
+  <si>
+    <t>IsHisto</t>
+  </si>
+  <si>
+    <t>HistoTestType</t>
+  </si>
+  <si>
+    <t>TestTitle,</t>
+  </si>
+  <si>
+    <t>TestParent,</t>
+  </si>
+  <si>
+    <t>DefaultResult</t>
+  </si>
+  <si>
+    <t>from tbl_HistoReportTypeLookUp</t>
+  </si>
+  <si>
+    <t>Histo</t>
+  </si>
+  <si>
+    <t>IsDifferentialTest</t>
+  </si>
+  <si>
+    <t>FFTestDiagnosis</t>
+  </si>
+  <si>
+    <t>DiagID</t>
+  </si>
+  <si>
+    <t>TestID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,8 +334,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,8 +368,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -303,11 +429,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -315,6 +452,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,6 +552,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -443,6 +604,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -621,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,19 +877,19 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="11" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -732,19 +910,19 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -765,16 +943,16 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="1"/>
@@ -796,10 +974,10 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="12" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="1"/>
@@ -821,10 +999,10 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="12" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="1"/>
@@ -846,10 +1024,10 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="1"/>
@@ -869,10 +1047,10 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="1"/>
@@ -890,10 +1068,10 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="12" t="s">
         <v>29</v>
       </c>
       <c r="G11" s="1"/>
@@ -909,10 +1087,10 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="1"/>
@@ -926,10 +1104,10 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="12" t="s">
         <v>30</v>
       </c>
       <c r="G13" s="1"/>
@@ -943,7 +1121,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="1"/>
@@ -958,7 +1136,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="12" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="1"/>
@@ -973,7 +1151,7 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="12" t="s">
         <v>21</v>
       </c>
       <c r="F16" s="1"/>
@@ -988,7 +1166,7 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="12" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="1"/>
@@ -1003,7 +1181,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="12" t="s">
         <v>23</v>
       </c>
       <c r="F18" s="1"/>
@@ -1018,7 +1196,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="1"/>
@@ -1033,7 +1211,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="12" t="s">
         <v>25</v>
       </c>
       <c r="F20" s="1"/>
@@ -1048,7 +1226,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="12" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="1"/>
@@ -1102,7 +1280,7 @@
       <c r="E24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1117,7 +1295,7 @@
       <c r="E25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1132,7 +1310,7 @@
       <c r="E26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="11" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1145,9 +1323,10 @@
       <c r="E27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="11" t="s">
         <v>65</v>
       </c>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -1156,7 +1335,7 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="13" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1167,7 +1346,7 @@
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="13" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1178,7 +1357,7 @@
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="11" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1189,7 +1368,7 @@
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -1198,10 +1377,337 @@
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="F32" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:L34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C16" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+    </row>
+    <row r="22" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+    </row>
+    <row r="23" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F28" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>92</v>
+      </c>
+      <c r="G33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>